<commit_message>
TechSpec Database and UI
</commit_message>
<xml_diff>
--- a/DropsTestRunDefinition.xlsx
+++ b/DropsTestRunDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5E66B5-404E-824A-92AA-957E47469EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D97911B-87A0-FA4A-A456-C5B594F250AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24640" yWindow="3080" windowWidth="26380" windowHeight="17760" activeTab="1" xr2:uid="{C21CBE73-8099-B346-9E91-2E7A276E3EDF}"/>
+    <workbookView xWindow="-25660" yWindow="1540" windowWidth="23940" windowHeight="17760" activeTab="2" xr2:uid="{C21CBE73-8099-B346-9E91-2E7A276E3EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="TestRun" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Attribute</t>
   </si>
@@ -322,9 +322,6 @@
     <t>CLICK</t>
   </si>
   <si>
-    <t>dummy</t>
-  </si>
-  <si>
     <t>TFName</t>
   </si>
   <si>
@@ -374,6 +371,12 @@
   </si>
   <si>
     <t>//button[contains(.,'Submit')]</t>
+  </si>
+  <si>
+    <t>LineNumbers</t>
+  </si>
+  <si>
+    <t>1:5, 6, 9, 11</t>
   </si>
 </sst>
 </file>
@@ -800,9 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F181D6E7-D17F-0041-A94D-64B92F668767}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -816,27 +817,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -874,9 +875,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2EF012-49BA-EB43-B0C5-88D33BAB0810}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -884,9 +885,11 @@
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -908,8 +911,11 @@
       <c r="G1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -917,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -930,6 +936,9 @@
       </c>
       <c r="G2">
         <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +951,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,7 +1008,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1032,7 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1037,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1059,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1095,13 +1104,13 @@
         <v>34</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
         <v>42</v>
-      </c>
-      <c r="M1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1121,7 +1130,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1144,10 +1153,10 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>49</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -1173,13 +1182,13 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1202,7 +1211,7 @@
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Path problems in UI-call (pyinstaller)
</commit_message>
<xml_diff>
--- a/DropsTestRunDefinition.xlsx
+++ b/DropsTestRunDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F849E8CF-BCF9-6146-A170-22FD68BDFDE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056FCED5-46B7-6A47-A1C5-A5229691F500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="3380" windowWidth="21440" windowHeight="18440" activeTab="2" xr2:uid="{C21CBE73-8099-B346-9E91-2E7A276E3EDF}"/>
+    <workbookView xWindow="7720" yWindow="2220" windowWidth="21440" windowHeight="18440" activeTab="5" xr2:uid="{C21CBE73-8099-B346-9E91-2E7A276E3EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="TestRun" sheetId="1" r:id="rId1"/>
@@ -334,9 +334,6 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>baangt.TestSteps.TestStepMaster</t>
-  </si>
-  <si>
     <t>Optional</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>DropsTestExample.xlsx</t>
+  </si>
+  <si>
+    <t>GC.CLASSES_TESTSTEPMASTER</t>
   </si>
 </sst>
 </file>
@@ -827,17 +827,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2EF012-49BA-EB43-B0C5-88D33BAB0810}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -912,7 +912,7 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -938,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -951,13 +951,14 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1008,7 +1009,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,7 +1033,7 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1046,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1058,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79890A34-1943-0E42-B53E-BE7CAA0D6A12}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1107,10 +1108,10 @@
         <v>38</v>
       </c>
       <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
         <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1130,7 +1131,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1153,10 +1154,10 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
         <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -1182,10 +1183,10 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
         <v>39</v>
@@ -1211,7 +1212,7 @@
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed lines in Testsquence to new format
</commit_message>
<xml_diff>
--- a/DropsTestRunDefinition.xlsx
+++ b/DropsTestRunDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056FCED5-46B7-6A47-A1C5-A5229691F500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A781DA5B-F1FF-1A40-87F5-5D31CCC08D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="2220" windowWidth="21440" windowHeight="18440" activeTab="5" xr2:uid="{C21CBE73-8099-B346-9E91-2E7A276E3EDF}"/>
+    <workbookView xWindow="7720" yWindow="2220" windowWidth="21440" windowHeight="18440" activeTab="2" xr2:uid="{C21CBE73-8099-B346-9E91-2E7A276E3EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="TestRun" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Attribute</t>
   </si>
@@ -250,12 +250,6 @@
     <t>ParallelRuns</t>
   </si>
   <si>
-    <t>FromLine</t>
-  </si>
-  <si>
-    <t>ToLine</t>
-  </si>
-  <si>
     <t>TestCaseSequenceNumber</t>
   </si>
   <si>
@@ -367,16 +361,16 @@
     <t>//button[contains(.,'Submit')]</t>
   </si>
   <si>
-    <t>LineNumbers</t>
-  </si>
-  <si>
-    <t>1:5, 6, 9, 11</t>
-  </si>
-  <si>
     <t>DropsTestExample.xlsx</t>
   </si>
   <si>
     <t>GC.CLASSES_TESTSTEPMASTER</t>
+  </si>
+  <si>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>1-2</t>
   </si>
 </sst>
 </file>
@@ -447,11 +441,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -817,27 +812,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -847,7 +842,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -875,10 +870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2EF012-49BA-EB43-B0C5-88D33BAB0810}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,10 +881,10 @@
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -897,7 +892,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -906,16 +901,10 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -923,7 +912,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -931,13 +920,7 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F2" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -963,22 +946,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -989,13 +972,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1021,19 +1004,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1047,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1059,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79890A34-1943-0E42-B53E-BE7CAA0D6A12}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1075,43 +1058,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" t="s">
-        <v>40</v>
-      </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1128,10 +1111,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1148,16 +1131,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -1177,19 +1160,19 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1206,13 +1189,13 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>